<commit_message>
Added receptor to tracer name mapping
</commit_message>
<xml_diff>
--- a/receptor2tracer.xlsx
+++ b/receptor2tracer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stuart\Documents\ThalamicGradients\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{914F9B0E-319D-4B12-82D5-A7A130332C9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1AE8A4B-CABA-4B4B-B6E3-9487C4AA3FB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="12705" xr2:uid="{87C9A815-4331-4FAA-97FE-2EA0931FDB98}"/>
+    <workbookView xWindow="16680" yWindow="3660" windowWidth="21600" windowHeight="12705" xr2:uid="{87C9A815-4331-4FAA-97FE-2EA0931FDB98}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="119">
   <si>
     <t>5HT1a</t>
   </si>
@@ -362,6 +362,36 @@
   </si>
   <si>
     <t>smart</t>
+  </si>
+  <si>
+    <t>cumi101</t>
+  </si>
+  <si>
+    <t>way100635</t>
+  </si>
+  <si>
+    <t>az10419369</t>
+  </si>
+  <si>
+    <t>altanserin</t>
+  </si>
+  <si>
+    <t>cimbi36</t>
+  </si>
+  <si>
+    <t>sb207145</t>
+  </si>
+  <si>
+    <t>gsk21508</t>
+  </si>
+  <si>
+    <t>abp688</t>
+  </si>
+  <si>
+    <t>mrb</t>
+  </si>
+  <si>
+    <t>sch23390</t>
   </si>
 </sst>
 </file>
@@ -713,20 +743,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{056FB569-4D3A-4954-9DAF-4CD6D93B1348}">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>109</v>
       </c>
       <c r="C1" t="s">
         <v>2</v>
@@ -734,13 +764,16 @@
       <c r="D1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>110</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
@@ -748,13 +781,16 @@
       <c r="D2" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>111</v>
       </c>
       <c r="C3" t="s">
         <v>4</v>
@@ -762,8 +798,11 @@
       <c r="D3" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
@@ -776,8 +815,11 @@
       <c r="D4" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -790,13 +832,16 @@
       <c r="D5" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>112</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
@@ -804,13 +849,16 @@
       <c r="D6" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>113</v>
       </c>
       <c r="C7" t="s">
         <v>14</v>
@@ -818,8 +866,11 @@
       <c r="D7" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -832,13 +883,16 @@
       <c r="D8" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>114</v>
       </c>
       <c r="C9" t="s">
         <v>19</v>
@@ -846,13 +900,16 @@
       <c r="D9" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>115</v>
       </c>
       <c r="C10" t="s">
         <v>22</v>
@@ -860,8 +917,11 @@
       <c r="D10" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -874,8 +934,11 @@
       <c r="D11" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -888,8 +951,11 @@
       <c r="D12" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>23</v>
       </c>
@@ -902,8 +968,11 @@
       <c r="D13" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -916,8 +985,11 @@
       <c r="D14" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -930,8 +1002,11 @@
       <c r="D15" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -944,13 +1019,16 @@
       <c r="D16" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>34</v>
       </c>
       <c r="B17" t="s">
-        <v>35</v>
+        <v>118</v>
       </c>
       <c r="C17" t="s">
         <v>36</v>
@@ -958,8 +1036,11 @@
       <c r="D17" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>37</v>
       </c>
@@ -972,8 +1053,11 @@
       <c r="D18" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>37</v>
       </c>
@@ -986,8 +1070,11 @@
       <c r="D19" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -1000,8 +1087,11 @@
       <c r="D20" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>37</v>
       </c>
@@ -1014,8 +1104,11 @@
       <c r="D21" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>45</v>
       </c>
@@ -1028,8 +1121,11 @@
       <c r="D22" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>45</v>
       </c>
@@ -1042,8 +1138,11 @@
       <c r="D23" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>51</v>
       </c>
@@ -1056,8 +1155,11 @@
       <c r="D24" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>54</v>
       </c>
@@ -1070,8 +1172,11 @@
       <c r="D25" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>57</v>
       </c>
@@ -1084,8 +1189,11 @@
       <c r="D26" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>58</v>
       </c>
@@ -1098,8 +1206,11 @@
       <c r="D27" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>60</v>
       </c>
@@ -1112,8 +1223,11 @@
       <c r="D28" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>63</v>
       </c>
@@ -1126,8 +1240,11 @@
       <c r="D29" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>63</v>
       </c>
@@ -1140,13 +1257,16 @@
       <c r="D30" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>67</v>
       </c>
       <c r="B31" t="s">
-        <v>68</v>
+        <v>117</v>
       </c>
       <c r="C31" t="s">
         <v>27</v>
@@ -1154,13 +1274,16 @@
       <c r="D31" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>67</v>
       </c>
       <c r="B32" t="s">
-        <v>68</v>
+        <v>117</v>
       </c>
       <c r="C32" t="s">
         <v>33</v>
@@ -1168,8 +1291,11 @@
       <c r="D32" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>69</v>
       </c>
@@ -1182,8 +1308,11 @@
       <c r="D33" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>71</v>
       </c>
@@ -1196,8 +1325,11 @@
       <c r="D34" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>71</v>
       </c>
@@ -1210,8 +1342,11 @@
       <c r="D35" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>71</v>
       </c>
@@ -1224,8 +1359,11 @@
       <c r="D36" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>78</v>
       </c>
@@ -1238,8 +1376,11 @@
       <c r="D37" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>78</v>
       </c>
@@ -1252,19 +1393,25 @@
       <c r="D38" t="s">
         <v>107</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>78</v>
       </c>
       <c r="B39" t="s">
-        <v>79</v>
+        <v>116</v>
       </c>
       <c r="C39" t="s">
         <v>81</v>
       </c>
       <c r="D39" t="s">
         <v>108</v>
+      </c>
+      <c r="E39" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>